<commit_message>
Edit Testcase & Calcontext
</commit_message>
<xml_diff>
--- a/TestCaseCalculator.xlsx
+++ b/TestCaseCalculator.xlsx
@@ -18,15 +18,188 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="54">
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>1. Mở ứng dụng calculator</t>
+  </si>
+  <si>
+    <t>Test steps</t>
+  </si>
+  <si>
+    <t>1. Nhấn btn số thứ nhất</t>
+  </si>
+  <si>
+    <t>2. Nhấn btn số thứ hai</t>
+  </si>
+  <si>
+    <t>3. Nhấn btn chức năng</t>
+  </si>
+  <si>
+    <t>4. Nhấn btn "="</t>
+  </si>
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Number1</t>
+  </si>
+  <si>
+    <t>Number2</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>"+"</t>
+  </si>
+  <si>
+    <t>Hiển thị 0</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Hiển thị -1</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>"-"</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>Function button</t>
+  </si>
+  <si>
+    <t>Hiển thị -2</t>
+  </si>
+  <si>
+    <t>"X"</t>
+  </si>
+  <si>
+    <t>"/"</t>
+  </si>
+  <si>
+    <t>Cộng 2 số nguyên</t>
+  </si>
+  <si>
+    <t>Hiển thị 1</t>
+  </si>
+  <si>
+    <t>Cộng 2 số thực</t>
+  </si>
+  <si>
+    <t>Hiển thị 1.2</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>Hiển thị -2.2</t>
+  </si>
+  <si>
+    <t>Trừ 2 số nguyên</t>
+  </si>
+  <si>
+    <t>Trừ 2 số thực</t>
+  </si>
+  <si>
+    <t>Hiển thị 2</t>
+  </si>
+  <si>
+    <t>Nhân 2 số nguyên</t>
+  </si>
+  <si>
+    <t>Nhân 2 số thực</t>
+  </si>
+  <si>
+    <t>Hiển thị 0.11</t>
+  </si>
+  <si>
+    <t>Hiển thị -1.21</t>
+  </si>
+  <si>
+    <t>Hiển thị 1.21</t>
+  </si>
+  <si>
+    <t>Chia 2 số nguyên</t>
+  </si>
+  <si>
+    <t>Chia 2 số thực</t>
+  </si>
+  <si>
+    <t>Hiển thị 2.2</t>
+  </si>
+  <si>
+    <t>Hiển thị 11</t>
+  </si>
+  <si>
+    <t>Hiển thị Error</t>
+  </si>
+  <si>
+    <t>Hiển thị 0.09090909090909091</t>
+  </si>
+  <si>
+    <t>Phần trăm số nguyên</t>
+  </si>
+  <si>
+    <t>Phần trăm số thực</t>
+  </si>
+  <si>
+    <t>"%"</t>
+  </si>
+  <si>
+    <t>Hiển thị 0.01</t>
+  </si>
+  <si>
+    <t>Hiển thị -0.01</t>
+  </si>
+  <si>
+    <t>Hiển thị 0.011000000000000001</t>
+  </si>
+  <si>
+    <t>Hiển thị 0.001</t>
+  </si>
+  <si>
+    <t>Hiển thị -0.011000000000000001</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +222,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +505,853 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G8">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G9">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <v>-1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G18">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G19">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>-1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24">
+        <v>-1</v>
+      </c>
+      <c r="G24">
+        <v>-1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26">
+        <v>-1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G28">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G29">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>-1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>-1</v>
+      </c>
+      <c r="G34">
+        <v>-1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36">
+        <v>-1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37">
+        <v>0.1</v>
+      </c>
+      <c r="G37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G38">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G39">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G40">
+        <v>0.1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="G41">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44">
+        <v>-1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H45" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46">
+        <v>0.1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>48</v>
+      </c>
+      <c r="I47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>